<commit_message>
US-13049 [FIX] TKC-KCL Comparison: Fixed row height
Signed-off-by: Dorian Kemps <dk@tempo-consulting.fr>
</commit_message>
<xml_diff>
--- a/bin/addons/kit/report/tkc_kcl_comparison_report.xlsx
+++ b/bin/addons/kit/report/tkc_kcl_comparison_report.xlsx
@@ -217,7 +217,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[Black]\+0;[Red]\-0;[Black]0"/>
+    <numFmt numFmtId="164" formatCode="[Black]\+0;[Red]\-0;[Black]0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -408,9 +408,30 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -426,32 +447,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -735,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,170 +753,172 @@
     <col min="15" max="16" width="11.28515625" customWidth="1"/>
     <col min="17" max="17" width="5.7109375" customWidth="1"/>
     <col min="18" max="18" width="5.85546875" customWidth="1"/>
-    <col min="19" max="22" width="5.7109375" customWidth="1"/>
+    <col min="19" max="19" width="5.7109375" customWidth="1"/>
+    <col min="20" max="21" width="7.7109375" customWidth="1"/>
+    <col min="22" max="22" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="26">
+      <c r="B2" s="27">
         <v>46042</v>
       </c>
-      <c r="C2" s="26"/>
+      <c r="C2" s="27"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="21"/>
+      <c r="C5" s="26"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="21"/>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="29"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="21"/>
+      <c r="C8" s="26"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
     </row>
     <row r="10" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="21"/>
+      <c r="C13" s="26"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="21"/>
+      <c r="C14" s="26"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="21"/>
+      <c r="C15" s="26"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="22"/>
+      <c r="C16" s="29"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="22"/>
+      <c r="C17" s="29"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
     </row>
     <row r="19" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
     </row>
     <row r="21" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="30"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B22" s="33"/>
+      <c r="C22" s="34"/>
+    </row>
+    <row r="23" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="30"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="34"/>
     </row>
     <row r="25" spans="1:21" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
@@ -958,7 +960,7 @@
       <c r="M25" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="N25" s="31" t="s">
+      <c r="N25" s="22" t="s">
         <v>25</v>
       </c>
       <c r="O25" s="3" t="s">
@@ -983,7 +985,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:21" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>34</v>
       </c>
@@ -1015,7 +1017,7 @@
       <c r="M26" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N26" s="34">
+      <c r="N26" s="25">
         <v>0</v>
       </c>
       <c r="O26" s="4" t="s">
@@ -1032,7 +1034,7 @@
       </c>
       <c r="U26" s="4"/>
     </row>
-    <row r="27" spans="1:21" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>34</v>
       </c>
@@ -1077,7 +1079,7 @@
       </c>
       <c r="U27" s="5"/>
     </row>
-    <row r="28" spans="1:21" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>38</v>
       </c>
@@ -1105,7 +1107,7 @@
       <c r="K28" s="8"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
-      <c r="N28" s="34">
+      <c r="N28" s="25">
         <v>0</v>
       </c>
       <c r="O28" s="4" t="s">
@@ -1122,7 +1124,7 @@
       </c>
       <c r="U28" s="4"/>
     </row>
-    <row r="29" spans="1:21" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>38</v>
       </c>
@@ -1169,7 +1171,7 @@
       </c>
       <c r="U29" s="5"/>
     </row>
-    <row r="30" spans="1:21" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>38</v>
       </c>
@@ -1216,7 +1218,7 @@
       </c>
       <c r="U30" s="5"/>
     </row>
-    <row r="31" spans="1:21" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>42</v>
       </c>
@@ -1244,7 +1246,7 @@
       <c r="K31" s="8"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
-      <c r="N31" s="33">
+      <c r="N31" s="24">
         <v>-1800</v>
       </c>
       <c r="O31" s="4" t="s">
@@ -1261,7 +1263,7 @@
       </c>
       <c r="U31" s="4"/>
     </row>
-    <row r="32" spans="1:21" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>42</v>
       </c>
@@ -1330,7 +1332,7 @@
       <c r="K33" s="13"/>
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
-      <c r="N33" s="32">
+      <c r="N33" s="23">
         <v>1000</v>
       </c>
       <c r="O33" s="9" t="s">
@@ -1384,6 +1386,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -1396,14 +1406,6 @@
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
US-13049 [FIX] TKC-KCL Comparison: Changed KCL header color, header deviations texts and kit items ordering
Signed-off-by: Dorian Kemps <dk@tempo-consulting.fr>
</commit_message>
<xml_diff>
--- a/bin/addons/kit/report/tkc_kcl_comparison_report.xlsx
+++ b/bin/addons/kit/report/tkc_kcl_comparison_report.xlsx
@@ -216,8 +216,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[Black]\+0;[Red]\-0;[Black]0"/>
+    <numFmt numFmtId="166" formatCode="[Black]\+0%;[Red]\-0%;[Black]0%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -251,7 +252,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,6 +292,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -348,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -396,9 +403,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -423,6 +427,9 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -451,6 +458,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -736,7 +749,7 @@
   <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="B22" sqref="B22:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,14 +920,16 @@
       <c r="C21" s="32"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="34"/>
+      <c r="B22" s="35">
+        <v>-0.25</v>
+      </c>
+      <c r="C22" s="36"/>
     </row>
     <row r="23" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="18" t="s">
         <v>59</v>
       </c>
       <c r="B23" s="33"/>
@@ -924,43 +939,43 @@
       <c r="A25" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="17" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="20" t="s">
+      <c r="E25" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="F25" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="G25" s="17" t="s">
+      <c r="G25" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="H25" s="17" t="s">
+      <c r="H25" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="I25" s="17" t="s">
+      <c r="I25" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="J25" s="17" t="s">
+      <c r="J25" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="K25" s="17" t="s">
+      <c r="K25" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="L25" s="17" t="s">
+      <c r="L25" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="M25" s="17" t="s">
+      <c r="M25" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="N25" s="22" t="s">
+      <c r="N25" s="21" t="s">
         <v>25</v>
       </c>
       <c r="O25" s="3" t="s">
@@ -985,7 +1000,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:21" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>34</v>
       </c>
@@ -1017,7 +1032,7 @@
       <c r="M26" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N26" s="25">
+      <c r="N26" s="24">
         <v>0</v>
       </c>
       <c r="O26" s="4" t="s">
@@ -1034,7 +1049,7 @@
       </c>
       <c r="U26" s="4"/>
     </row>
-    <row r="27" spans="1:21" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>34</v>
       </c>
@@ -1079,7 +1094,7 @@
       </c>
       <c r="U27" s="5"/>
     </row>
-    <row r="28" spans="1:21" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>38</v>
       </c>
@@ -1107,7 +1122,7 @@
       <c r="K28" s="8"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
-      <c r="N28" s="25">
+      <c r="N28" s="24">
         <v>0</v>
       </c>
       <c r="O28" s="4" t="s">
@@ -1124,7 +1139,7 @@
       </c>
       <c r="U28" s="4"/>
     </row>
-    <row r="29" spans="1:21" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>38</v>
       </c>
@@ -1171,7 +1186,7 @@
       </c>
       <c r="U29" s="5"/>
     </row>
-    <row r="30" spans="1:21" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>38</v>
       </c>
@@ -1218,7 +1233,7 @@
       </c>
       <c r="U30" s="5"/>
     </row>
-    <row r="31" spans="1:21" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>42</v>
       </c>
@@ -1246,7 +1261,7 @@
       <c r="K31" s="8"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
-      <c r="N31" s="24">
+      <c r="N31" s="23">
         <v>-1800</v>
       </c>
       <c r="O31" s="4" t="s">
@@ -1263,7 +1278,7 @@
       </c>
       <c r="U31" s="4"/>
     </row>
-    <row r="32" spans="1:21" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>42</v>
       </c>
@@ -1332,7 +1347,7 @@
       <c r="K33" s="13"/>
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
-      <c r="N33" s="23">
+      <c r="N33" s="22">
         <v>1000</v>
       </c>
       <c r="O33" s="9" t="s">

</xml_diff>